<commit_message>
Update for women's NCAA tourney 2024.
</commit_message>
<xml_diff>
--- a/NCAA-bracket-pool/2024/report-w.xlsx
+++ b/NCAA-bracket-pool/2024/report-w.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/theodore_flynn_water_ca_gov/Documents/personal/ncaa_bracket_pool/2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\teds-code\NCAA-bracket-pool\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:40009_{2FDB973C-D44D-4E5C-A208-680F1178E336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5CA5684-8A47-43E7-A11D-B4E0421F1057}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D46409-E5A1-441A-9D7D-4F5C38F25E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10890" yWindow="2055" windowWidth="38010" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35100" yWindow="540" windowWidth="21600" windowHeight="15630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="report-w" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="176">
   <si>
     <t>A1R - R1 - G1</t>
   </si>
@@ -349,9 +349,6 @@
     <t>Princeton</t>
   </si>
   <si>
-    <t>Sacred Heart/Presbeterian</t>
-  </si>
-  <si>
     <t>Oklahoma</t>
   </si>
   <si>
@@ -367,15 +364,6 @@
     <t>Chattanooga</t>
   </si>
   <si>
-    <t>A&amp;M-Corpus Christi</t>
-  </si>
-  <si>
-    <t>Vanderbilt/Columbia</t>
-  </si>
-  <si>
-    <t>Auburn/Arizona</t>
-  </si>
-  <si>
     <t>Middle Tenn.</t>
   </si>
   <si>
@@ -403,15 +391,9 @@
     <t>West Virginia</t>
   </si>
   <si>
-    <t>Uconn</t>
-  </si>
-  <si>
     <t>Vanderbilt</t>
   </si>
   <si>
-    <t>Colorad</t>
-  </si>
-  <si>
     <t xml:space="preserve">South Carolina </t>
   </si>
   <si>
@@ -557,6 +539,15 @@
   </si>
   <si>
     <t>Scott Waller</t>
+  </si>
+  <si>
+    <t>Sacred Heart</t>
+  </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>Texas A&amp;M-Corpus Christi</t>
   </si>
 </sst>
 </file>
@@ -1419,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AO20" sqref="AO20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,7 +1438,7 @@
     <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="12" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="12" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="20" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -1469,7 +1460,7 @@
   <sheetData>
     <row r="1" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1663,13 +1654,13 @@
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
         <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
@@ -1678,7 +1669,7 @@
         <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G2" t="s">
         <v>65</v>
@@ -1696,7 +1687,7 @@
         <v>86</v>
       </c>
       <c r="L2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M2" t="s">
         <v>66</v>
@@ -1714,7 +1705,7 @@
         <v>68</v>
       </c>
       <c r="R2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S2" t="s">
         <v>69</v>
@@ -1741,7 +1732,7 @@
         <v>70</v>
       </c>
       <c r="AA2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AB2" t="s">
         <v>72</v>
@@ -1777,10 +1768,10 @@
         <v>79</v>
       </c>
       <c r="AM2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AO2" t="s">
         <v>75</v>
@@ -1792,7 +1783,7 @@
         <v>78</v>
       </c>
       <c r="AR2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AS2" t="s">
         <v>99</v>
@@ -1828,7 +1819,7 @@
         <v>80</v>
       </c>
       <c r="BD2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="BE2" t="s">
         <v>85</v>
@@ -1857,7 +1848,7 @@
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
         <v>86</v>
@@ -2051,10 +2042,10 @@
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
         <v>87</v>
@@ -2063,13 +2054,13 @@
         <v>63</v>
       </c>
       <c r="E4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" t="s">
         <v>110</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>111</v>
-      </c>
-      <c r="G4" t="s">
-        <v>112</v>
       </c>
       <c r="H4" t="s">
         <v>66</v>
@@ -2084,7 +2075,7 @@
         <v>87</v>
       </c>
       <c r="L4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M4" t="s">
         <v>66</v>
@@ -2093,7 +2084,7 @@
         <v>63</v>
       </c>
       <c r="O4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P4" t="s">
         <v>63</v>
@@ -2102,7 +2093,7 @@
         <v>92</v>
       </c>
       <c r="R4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S4" t="s">
         <v>69</v>
@@ -2114,7 +2105,7 @@
         <v>96</v>
       </c>
       <c r="V4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="W4" t="s">
         <v>97</v>
@@ -2132,7 +2123,7 @@
         <v>92</v>
       </c>
       <c r="AB4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AC4" t="s">
         <v>73</v>
@@ -2144,19 +2135,19 @@
         <v>95</v>
       </c>
       <c r="AF4" t="s">
-        <v>115</v>
+        <v>175</v>
       </c>
       <c r="AG4" t="s">
         <v>100</v>
       </c>
       <c r="AH4" t="s">
-        <v>116</v>
+        <v>174</v>
       </c>
       <c r="AI4" t="s">
         <v>76</v>
       </c>
       <c r="AJ4" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="AK4" t="s">
         <v>78</v>
@@ -2195,19 +2186,19 @@
         <v>81</v>
       </c>
       <c r="AW4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="AX4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="AY4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="AZ4" t="s">
         <v>81</v>
       </c>
       <c r="BA4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="BB4" t="s">
         <v>81</v>
@@ -2222,7 +2213,7 @@
         <v>85</v>
       </c>
       <c r="BF4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="BG4" t="s">
         <v>85</v>
@@ -2245,7 +2236,7 @@
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
         <v>86</v>
@@ -2257,10 +2248,10 @@
         <v>63</v>
       </c>
       <c r="E5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" t="s">
         <v>110</v>
-      </c>
-      <c r="F5" t="s">
-        <v>111</v>
       </c>
       <c r="G5" t="s">
         <v>65</v>
@@ -2278,7 +2269,7 @@
         <v>86</v>
       </c>
       <c r="L5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M5" t="s">
         <v>66</v>
@@ -2359,7 +2350,7 @@
         <v>79</v>
       </c>
       <c r="AM5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN5" t="s">
         <v>79</v>
@@ -2439,7 +2430,7 @@
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B6" t="s">
         <v>86</v>
@@ -2451,10 +2442,10 @@
         <v>63</v>
       </c>
       <c r="E6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
         <v>110</v>
-      </c>
-      <c r="F6" t="s">
-        <v>111</v>
       </c>
       <c r="G6" t="s">
         <v>65</v>
@@ -2466,7 +2457,7 @@
         <v>91</v>
       </c>
       <c r="J6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K6" t="s">
         <v>86</v>
@@ -2481,16 +2472,16 @@
         <v>86</v>
       </c>
       <c r="O6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="P6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="Q6" t="s">
         <v>68</v>
       </c>
       <c r="R6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S6" t="s">
         <v>69</v>
@@ -2505,7 +2496,7 @@
         <v>72</v>
       </c>
       <c r="W6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="X6" t="s">
         <v>73</v>
@@ -2553,10 +2544,10 @@
         <v>104</v>
       </c>
       <c r="AM6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AO6" t="s">
         <v>75</v>
@@ -2622,18 +2613,18 @@
         <v>85</v>
       </c>
       <c r="BJ6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="BK6" t="s">
         <v>81</v>
       </c>
       <c r="BL6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s">
         <v>86</v>
@@ -2645,13 +2636,13 @@
         <v>63</v>
       </c>
       <c r="E7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" t="s">
         <v>110</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>111</v>
-      </c>
-      <c r="G7" t="s">
-        <v>112</v>
       </c>
       <c r="H7" t="s">
         <v>66</v>
@@ -2666,7 +2657,7 @@
         <v>86</v>
       </c>
       <c r="L7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M7" t="s">
         <v>66</v>
@@ -2675,7 +2666,7 @@
         <v>86</v>
       </c>
       <c r="O7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P7" t="s">
         <v>86</v>
@@ -2684,7 +2675,7 @@
         <v>68</v>
       </c>
       <c r="R7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S7" t="s">
         <v>94</v>
@@ -2711,7 +2702,7 @@
         <v>70</v>
       </c>
       <c r="AA7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AB7" t="s">
         <v>72</v>
@@ -2720,10 +2711,10 @@
         <v>72</v>
       </c>
       <c r="AD7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AE7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF7" t="s">
         <v>99</v>
@@ -2747,10 +2738,10 @@
         <v>104</v>
       </c>
       <c r="AM7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AO7" t="s">
         <v>75</v>
@@ -2762,13 +2753,13 @@
         <v>77</v>
       </c>
       <c r="AR7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AS7" t="s">
         <v>99</v>
       </c>
       <c r="AT7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AU7" t="s">
         <v>81</v>
@@ -2827,22 +2818,22 @@
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
         <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
       </c>
       <c r="E8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" t="s">
         <v>110</v>
-      </c>
-      <c r="F8" t="s">
-        <v>111</v>
       </c>
       <c r="G8" t="s">
         <v>65</v>
@@ -2860,7 +2851,7 @@
         <v>86</v>
       </c>
       <c r="L8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M8" t="s">
         <v>66</v>
@@ -2941,10 +2932,10 @@
         <v>104</v>
       </c>
       <c r="AM8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AO8" t="s">
         <v>75</v>
@@ -2956,7 +2947,7 @@
         <v>78</v>
       </c>
       <c r="AR8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AS8" t="s">
         <v>99</v>
@@ -2992,7 +2983,7 @@
         <v>80</v>
       </c>
       <c r="BD8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="BE8" t="s">
         <v>85</v>
@@ -3021,22 +3012,22 @@
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
         <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
       </c>
       <c r="E9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" t="s">
         <v>110</v>
-      </c>
-      <c r="F9" t="s">
-        <v>111</v>
       </c>
       <c r="G9" t="s">
         <v>65</v>
@@ -3054,7 +3045,7 @@
         <v>86</v>
       </c>
       <c r="L9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M9" t="s">
         <v>66</v>
@@ -3135,10 +3126,10 @@
         <v>79</v>
       </c>
       <c r="AM9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AO9" t="s">
         <v>75</v>
@@ -3171,7 +3162,7 @@
         <v>83</v>
       </c>
       <c r="AY9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="AZ9" t="s">
         <v>81</v>
@@ -3186,7 +3177,7 @@
         <v>80</v>
       </c>
       <c r="BD9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="BE9" t="s">
         <v>85</v>
@@ -3215,7 +3206,7 @@
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B10" t="s">
         <v>86</v>
@@ -3227,13 +3218,13 @@
         <v>63</v>
       </c>
       <c r="E10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" t="s">
         <v>110</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>111</v>
-      </c>
-      <c r="G10" t="s">
-        <v>112</v>
       </c>
       <c r="H10" t="s">
         <v>66</v>
@@ -3248,7 +3239,7 @@
         <v>86</v>
       </c>
       <c r="L10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M10" t="s">
         <v>66</v>
@@ -3257,7 +3248,7 @@
         <v>86</v>
       </c>
       <c r="O10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P10" t="s">
         <v>86</v>
@@ -3281,7 +3272,7 @@
         <v>72</v>
       </c>
       <c r="W10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="X10" t="s">
         <v>73</v>
@@ -3329,10 +3320,10 @@
         <v>104</v>
       </c>
       <c r="AM10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AO10" t="s">
         <v>75</v>
@@ -3359,13 +3350,13 @@
         <v>81</v>
       </c>
       <c r="AW10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="AX10" t="s">
         <v>83</v>
       </c>
       <c r="AY10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="AZ10" t="s">
         <v>81</v>
@@ -3409,7 +3400,7 @@
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
         <v>86</v>
@@ -3421,10 +3412,10 @@
         <v>63</v>
       </c>
       <c r="E11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" t="s">
         <v>110</v>
-      </c>
-      <c r="F11" t="s">
-        <v>111</v>
       </c>
       <c r="G11" t="s">
         <v>65</v>
@@ -3460,7 +3451,7 @@
         <v>68</v>
       </c>
       <c r="R11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S11" t="s">
         <v>69</v>
@@ -3523,10 +3514,10 @@
         <v>104</v>
       </c>
       <c r="AM11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AO11" t="s">
         <v>75</v>
@@ -3538,13 +3529,13 @@
         <v>77</v>
       </c>
       <c r="AR11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AS11" t="s">
         <v>75</v>
       </c>
       <c r="AT11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AU11" t="s">
         <v>80</v>
@@ -3559,10 +3550,10 @@
         <v>83</v>
       </c>
       <c r="AY11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="AZ11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="BA11" t="s">
         <v>83</v>
@@ -3574,7 +3565,7 @@
         <v>80</v>
       </c>
       <c r="BD11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="BE11" t="s">
         <v>85</v>
@@ -3603,22 +3594,22 @@
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s">
         <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
         <v>63</v>
       </c>
       <c r="E12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" t="s">
         <v>110</v>
-      </c>
-      <c r="F12" t="s">
-        <v>111</v>
       </c>
       <c r="G12" t="s">
         <v>65</v>
@@ -3636,7 +3627,7 @@
         <v>86</v>
       </c>
       <c r="L12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M12" t="s">
         <v>66</v>
@@ -3654,7 +3645,7 @@
         <v>68</v>
       </c>
       <c r="R12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S12" t="s">
         <v>69</v>
@@ -3669,7 +3660,7 @@
         <v>72</v>
       </c>
       <c r="W12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="X12" t="s">
         <v>73</v>
@@ -3717,10 +3708,10 @@
         <v>79</v>
       </c>
       <c r="AM12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AP12" t="s">
         <v>99</v>
@@ -3794,22 +3785,22 @@
     </row>
     <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s">
         <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D13" t="s">
         <v>63</v>
       </c>
       <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" t="s">
         <v>110</v>
-      </c>
-      <c r="F13" t="s">
-        <v>111</v>
       </c>
       <c r="G13" t="s">
         <v>65</v>
@@ -3827,7 +3818,7 @@
         <v>86</v>
       </c>
       <c r="L13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M13" t="s">
         <v>66</v>
@@ -3836,7 +3827,7 @@
         <v>86</v>
       </c>
       <c r="O13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P13" t="s">
         <v>86</v>
@@ -3908,10 +3899,10 @@
         <v>79</v>
       </c>
       <c r="AM13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AO13" t="s">
         <v>75</v>
@@ -3923,7 +3914,7 @@
         <v>78</v>
       </c>
       <c r="AR13" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="AS13" t="s">
         <v>99</v>
@@ -3988,7 +3979,7 @@
     </row>
     <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B14" t="s">
         <v>86</v>
@@ -4000,13 +3991,13 @@
         <v>88</v>
       </c>
       <c r="E14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
         <v>110</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>111</v>
-      </c>
-      <c r="G14" t="s">
-        <v>112</v>
       </c>
       <c r="H14" t="s">
         <v>66</v>
@@ -4015,13 +4006,13 @@
         <v>91</v>
       </c>
       <c r="J14" t="s">
+        <v>109</v>
+      </c>
+      <c r="K14" t="s">
+        <v>86</v>
+      </c>
+      <c r="L14" t="s">
         <v>110</v>
-      </c>
-      <c r="K14" t="s">
-        <v>86</v>
-      </c>
-      <c r="L14" t="s">
-        <v>111</v>
       </c>
       <c r="M14" t="s">
         <v>66</v>
@@ -4039,7 +4030,7 @@
         <v>68</v>
       </c>
       <c r="R14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S14" t="s">
         <v>69</v>
@@ -4051,7 +4042,7 @@
         <v>71</v>
       </c>
       <c r="V14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="W14" t="s">
         <v>97</v>
@@ -4102,10 +4093,10 @@
         <v>79</v>
       </c>
       <c r="AM14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AO14" t="s">
         <v>75</v>
@@ -4117,7 +4108,7 @@
         <v>78</v>
       </c>
       <c r="AR14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AS14" t="s">
         <v>99</v>
@@ -4138,7 +4129,7 @@
         <v>83</v>
       </c>
       <c r="AY14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="AZ14" t="s">
         <v>81</v>
@@ -4153,7 +4144,7 @@
         <v>80</v>
       </c>
       <c r="BD14" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="BE14" t="s">
         <v>85</v>
@@ -4182,7 +4173,7 @@
     </row>
     <row r="15" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s">
         <v>86</v>
@@ -4194,10 +4185,10 @@
         <v>88</v>
       </c>
       <c r="E15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" t="s">
         <v>110</v>
-      </c>
-      <c r="F15" t="s">
-        <v>111</v>
       </c>
       <c r="G15" t="s">
         <v>65</v>
@@ -4209,13 +4200,13 @@
         <v>91</v>
       </c>
       <c r="J15" t="s">
+        <v>109</v>
+      </c>
+      <c r="K15" t="s">
+        <v>86</v>
+      </c>
+      <c r="L15" t="s">
         <v>110</v>
-      </c>
-      <c r="K15" t="s">
-        <v>86</v>
-      </c>
-      <c r="L15" t="s">
-        <v>111</v>
       </c>
       <c r="M15" t="s">
         <v>66</v>
@@ -4296,10 +4287,10 @@
         <v>104</v>
       </c>
       <c r="AM15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AO15" t="s">
         <v>75</v>
@@ -4326,7 +4317,7 @@
         <v>81</v>
       </c>
       <c r="AW15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="AX15" t="s">
         <v>83</v>
@@ -4353,10 +4344,10 @@
         <v>85</v>
       </c>
       <c r="BF15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="BG15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="BH15" t="s">
         <v>80</v>
@@ -4376,7 +4367,7 @@
     </row>
     <row r="16" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B16" t="s">
         <v>86</v>
@@ -4388,10 +4379,10 @@
         <v>63</v>
       </c>
       <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
         <v>110</v>
-      </c>
-      <c r="F16" t="s">
-        <v>111</v>
       </c>
       <c r="G16" t="s">
         <v>65</v>
@@ -4427,7 +4418,7 @@
         <v>68</v>
       </c>
       <c r="R16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S16" t="s">
         <v>94</v>
@@ -4439,7 +4430,7 @@
         <v>96</v>
       </c>
       <c r="V16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="W16" t="s">
         <v>97</v>
@@ -4475,7 +4466,7 @@
         <v>100</v>
       </c>
       <c r="AH16" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="AI16" t="s">
         <v>76</v>
@@ -4490,10 +4481,10 @@
         <v>79</v>
       </c>
       <c r="AM16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AO16" t="s">
         <v>76</v>
@@ -4505,16 +4496,16 @@
         <v>77</v>
       </c>
       <c r="AR16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AS16" t="s">
         <v>100</v>
       </c>
       <c r="AT16" t="s">
+        <v>118</v>
+      </c>
+      <c r="AU16" t="s">
         <v>122</v>
-      </c>
-      <c r="AU16" t="s">
-        <v>126</v>
       </c>
       <c r="AV16" t="s">
         <v>81</v>
@@ -4541,51 +4532,51 @@
         <v>80</v>
       </c>
       <c r="BD16" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="BE16" t="s">
         <v>85</v>
       </c>
       <c r="BF16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="BG16" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="BH16" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="BI16" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="BJ16" t="s">
         <v>63</v>
       </c>
       <c r="BK16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="BL16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s">
         <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D17" t="s">
         <v>63</v>
       </c>
       <c r="E17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" t="s">
         <v>110</v>
-      </c>
-      <c r="F17" t="s">
-        <v>111</v>
       </c>
       <c r="G17" t="s">
         <v>65</v>
@@ -4597,13 +4588,13 @@
         <v>91</v>
       </c>
       <c r="J17" t="s">
+        <v>109</v>
+      </c>
+      <c r="K17" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" t="s">
         <v>110</v>
-      </c>
-      <c r="K17" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" t="s">
-        <v>111</v>
       </c>
       <c r="M17" t="s">
         <v>66</v>
@@ -4669,7 +4660,7 @@
         <v>74</v>
       </c>
       <c r="AH17" t="s">
-        <v>116</v>
+        <v>174</v>
       </c>
       <c r="AI17" t="s">
         <v>76</v>
@@ -4684,10 +4675,10 @@
         <v>79</v>
       </c>
       <c r="AM17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AN17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AO17" t="s">
         <v>76</v>
@@ -4699,7 +4690,7 @@
         <v>78</v>
       </c>
       <c r="AR17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AS17" t="s">
         <v>99</v>
@@ -4708,34 +4699,34 @@
         <v>99</v>
       </c>
       <c r="AU17" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="AV17" t="s">
         <v>81</v>
       </c>
       <c r="AW17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="AX17" t="s">
         <v>83</v>
       </c>
       <c r="AY17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="AZ17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="BA17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="BB17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="BC17" t="s">
         <v>80</v>
       </c>
       <c r="BD17" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="BE17" t="s">
         <v>107</v>
@@ -4747,10 +4738,10 @@
         <v>106</v>
       </c>
       <c r="BH17" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="BI17" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="BJ17" t="s">
         <v>86</v>
@@ -4764,196 +4755,196 @@
     </row>
     <row r="18" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" t="s">
+        <v>128</v>
+      </c>
+      <c r="G18" t="s">
+        <v>129</v>
+      </c>
+      <c r="H18" t="s">
+        <v>119</v>
+      </c>
+      <c r="I18" t="s">
         <v>130</v>
-      </c>
-      <c r="C18" t="s">
-        <v>131</v>
-      </c>
-      <c r="D18" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18" t="s">
-        <v>133</v>
-      </c>
-      <c r="F18" t="s">
-        <v>134</v>
-      </c>
-      <c r="G18" t="s">
-        <v>135</v>
-      </c>
-      <c r="H18" t="s">
-        <v>123</v>
-      </c>
-      <c r="I18" t="s">
-        <v>136</v>
       </c>
       <c r="J18" t="s">
         <v>63</v>
       </c>
       <c r="K18" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="L18" t="s">
+        <v>128</v>
+      </c>
+      <c r="M18" t="s">
+        <v>119</v>
+      </c>
+      <c r="N18" t="s">
+        <v>124</v>
+      </c>
+      <c r="O18" t="s">
+        <v>119</v>
+      </c>
+      <c r="P18" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>131</v>
+      </c>
+      <c r="R18" t="s">
+        <v>132</v>
+      </c>
+      <c r="S18" t="s">
+        <v>133</v>
+      </c>
+      <c r="T18" t="s">
         <v>134</v>
       </c>
-      <c r="M18" t="s">
-        <v>123</v>
-      </c>
-      <c r="N18" t="s">
-        <v>130</v>
-      </c>
-      <c r="O18" t="s">
-        <v>123</v>
-      </c>
-      <c r="P18" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q18" t="s">
+      <c r="U18" t="s">
+        <v>135</v>
+      </c>
+      <c r="V18" t="s">
+        <v>136</v>
+      </c>
+      <c r="W18" t="s">
         <v>137</v>
       </c>
-      <c r="R18" t="s">
+      <c r="X18" t="s">
         <v>138</v>
       </c>
-      <c r="S18" t="s">
+      <c r="Y18" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF18" t="s">
         <v>139</v>
       </c>
-      <c r="T18" t="s">
+      <c r="AG18" t="s">
         <v>140</v>
       </c>
-      <c r="U18" t="s">
+      <c r="AH18" t="s">
         <v>141</v>
       </c>
-      <c r="V18" t="s">
+      <c r="AI18" t="s">
         <v>142</v>
       </c>
-      <c r="W18" t="s">
+      <c r="AJ18" t="s">
         <v>143</v>
       </c>
-      <c r="X18" t="s">
+      <c r="AK18" t="s">
         <v>144</v>
       </c>
-      <c r="Y18" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>137</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>144</v>
-      </c>
-      <c r="AF18" t="s">
+      <c r="AL18" t="s">
         <v>145</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AM18" t="s">
         <v>146</v>
       </c>
-      <c r="AH18" t="s">
-        <v>147</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>148</v>
-      </c>
-      <c r="AJ18" t="s">
-        <v>149</v>
-      </c>
-      <c r="AK18" t="s">
-        <v>150</v>
-      </c>
-      <c r="AL18" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM18" t="s">
-        <v>152</v>
-      </c>
       <c r="AN18" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="AO18" t="s">
         <v>75</v>
       </c>
       <c r="AP18" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="AQ18" t="s">
+        <v>144</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>146</v>
+      </c>
+      <c r="AS18" t="s">
+        <v>139</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>139</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV18" t="s">
+        <v>148</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>149</v>
+      </c>
+      <c r="AX18" t="s">
         <v>150</v>
       </c>
-      <c r="AR18" t="s">
+      <c r="AY18" t="s">
+        <v>151</v>
+      </c>
+      <c r="AZ18" t="s">
+        <v>148</v>
+      </c>
+      <c r="BA18" t="s">
+        <v>150</v>
+      </c>
+      <c r="BB18" t="s">
+        <v>150</v>
+      </c>
+      <c r="BC18" t="s">
+        <v>147</v>
+      </c>
+      <c r="BD18" t="s">
         <v>152</v>
       </c>
-      <c r="AS18" t="s">
-        <v>145</v>
-      </c>
-      <c r="AT18" t="s">
-        <v>145</v>
-      </c>
-      <c r="AU18" t="s">
+      <c r="BE18" t="s">
         <v>153</v>
       </c>
-      <c r="AV18" t="s">
+      <c r="BF18" t="s">
         <v>154</v>
       </c>
-      <c r="AW18" t="s">
-        <v>155</v>
-      </c>
-      <c r="AX18" t="s">
-        <v>156</v>
-      </c>
-      <c r="AY18" t="s">
-        <v>157</v>
-      </c>
-      <c r="AZ18" t="s">
-        <v>154</v>
-      </c>
-      <c r="BA18" t="s">
-        <v>156</v>
-      </c>
-      <c r="BB18" t="s">
-        <v>156</v>
-      </c>
-      <c r="BC18" t="s">
+      <c r="BG18" t="s">
         <v>153</v>
       </c>
-      <c r="BD18" t="s">
-        <v>158</v>
-      </c>
-      <c r="BE18" t="s">
-        <v>159</v>
-      </c>
-      <c r="BF18" t="s">
-        <v>160</v>
-      </c>
-      <c r="BG18" t="s">
-        <v>159</v>
-      </c>
       <c r="BH18" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="BI18" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="BJ18" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="BK18" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="BL18" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>